<commit_message>
feat: demo_ prefix for IDATs
</commit_message>
<xml_diff>
--- a/EpiSign-METRIC_demo_patient_data.xlsx
+++ b/EpiSign-METRIC_demo_patient_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/episign/git/EpiSign-METRIC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C4E1691-EBAD-CE4E-A7FA-36A18B5EF9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69F5F00-1904-024B-A492-D3BF812308AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="3320" windowWidth="26040" windowHeight="14940" xr2:uid="{16A5A983-3C56-734A-BD02-C3ACE3E62644}"/>
   </bookViews>
@@ -44,24 +44,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>GSM3572694_202702320174_R07C01</t>
-  </si>
-  <si>
-    <t>GSM3572717_202702240172_R08C01</t>
-  </si>
-  <si>
-    <t>GSM3572721_202702320243_R07C01</t>
-  </si>
-  <si>
-    <t>GSM3400675_O1</t>
-  </si>
-  <si>
-    <t>GSM3572692_202702240101_R04C01</t>
-  </si>
-  <si>
-    <t>GSM3572693_202702240017_R05C01</t>
-  </si>
-  <si>
     <t>TBRS</t>
   </si>
   <si>
@@ -78,6 +60,24 @@
   </si>
   <si>
     <t>NCBRS</t>
+  </si>
+  <si>
+    <t>demo_GSM3572717_202702240172_R08C01</t>
+  </si>
+  <si>
+    <t>demo_GSM3572721_202702320243_R07C01</t>
+  </si>
+  <si>
+    <t>demo_GSM3400675_O1</t>
+  </si>
+  <si>
+    <t>demo_GSM3572692_202702240101_R04C01</t>
+  </si>
+  <si>
+    <t>demo_GSM3572693_202702240017_R05C01</t>
+  </si>
+  <si>
+    <t>demo_GSM3572694_202702320174_R07C01</t>
   </si>
 </sst>
 </file>
@@ -452,12 +452,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -470,50 +470,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>